<commit_message>
Excel inventory page update..
</commit_message>
<xml_diff>
--- a/script/af gastos 2013 11.xlsx
+++ b/script/af gastos 2013 11.xlsx
@@ -4338,10 +4338,10 @@
   <dimension ref="A1:T599"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D284" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C288" sqref="C288"/>
+      <selection pane="bottomRight" activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="11.25"/>
@@ -17735,7 +17735,7 @@
       <c r="B223" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C223" s="1" t="s">
+      <c r="C223" s="17" t="s">
         <v>448</v>
       </c>
       <c r="D223" s="1">

</xml_diff>

<commit_message>
Adding show number pages in Paginator class.
</commit_message>
<xml_diff>
--- a/script/af gastos 2013 11.xlsx
+++ b/script/af gastos 2013 11.xlsx
@@ -4338,10 +4338,10 @@
   <dimension ref="A1:T599"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D240" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D335" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A244" sqref="A244"/>
+      <selection pane="bottomRight" activeCell="A339" sqref="A339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="11.25"/>
@@ -21029,7 +21029,7 @@
       <c r="B277" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C277" s="1" t="s">
+      <c r="C277" s="17" t="s">
         <v>258</v>
       </c>
       <c r="D277" s="1">
@@ -21151,7 +21151,7 @@
       <c r="B279" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C279" s="1" t="s">
+      <c r="C279" s="17" t="s">
         <v>258</v>
       </c>
       <c r="D279" s="1">
@@ -24589,7 +24589,7 @@
       <c r="B338" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C338" s="1" t="s">
+      <c r="C338" s="17" t="s">
         <v>895</v>
       </c>
       <c r="D338" s="1">
@@ -24650,7 +24650,7 @@
       <c r="B339" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C339" s="1" t="s">
+      <c r="C339" s="17" t="s">
         <v>897</v>
       </c>
       <c r="D339" s="1">
@@ -24772,7 +24772,7 @@
       <c r="B341" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C341" s="1" t="s">
+      <c r="C341" s="17" t="s">
         <v>901</v>
       </c>
       <c r="D341" s="1">
@@ -25016,7 +25016,7 @@
       <c r="B345" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C345" s="1" t="s">
+      <c r="C345" s="17" t="s">
         <v>909</v>
       </c>
       <c r="D345" s="1">
@@ -29774,7 +29774,7 @@
       <c r="B423" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="C423" s="1" t="s">
+      <c r="C423" s="17" t="s">
         <v>701</v>
       </c>
       <c r="D423" s="1">

</xml_diff>

<commit_message>
Paginator little changes. Day finished.
</commit_message>
<xml_diff>
--- a/script/af gastos 2013 11.xlsx
+++ b/script/af gastos 2013 11.xlsx
@@ -4341,10 +4341,10 @@
   <dimension ref="A1:T599"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D215" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D340" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A219" sqref="A219"/>
+      <selection pane="bottomRight" activeCell="A344" sqref="A344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="11.25"/>
@@ -11064,7 +11064,7 @@
       <c r="B113" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="17" t="s">
         <v>497</v>
       </c>
       <c r="D113" s="1">
@@ -18409,7 +18409,7 @@
       <c r="B234" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C234" s="1" t="s">
+      <c r="C234" s="17" t="s">
         <v>331</v>
       </c>
       <c r="D234" s="1">
@@ -20849,7 +20849,7 @@
       <c r="B274" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C274" s="1" t="s">
+      <c r="C274" s="17" t="s">
         <v>247</v>
       </c>
       <c r="D274" s="1">
@@ -24958,7 +24958,7 @@
       <c r="B344" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C344" s="1" t="s">
+      <c r="C344" s="17" t="s">
         <v>907</v>
       </c>
       <c r="D344" s="1">
@@ -27337,7 +27337,7 @@
       <c r="B383" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C383" s="1" t="s">
+      <c r="C383" s="17" t="s">
         <v>801</v>
       </c>
       <c r="D383" s="1">
@@ -35918,7 +35918,7 @@
       <c r="B528" s="1" t="s">
         <v>981</v>
       </c>
-      <c r="C528" s="1" t="s">
+      <c r="C528" s="19" t="s">
         <v>982</v>
       </c>
       <c r="D528" s="1">

</xml_diff>